<commit_message>
UPDATE: DATA 24 Maret 2020
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FD380D-8575-40BB-B8A4-4D52C5080960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C49C4E7-33A5-4D78-9FA8-D312D441AB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="3315" windowWidth="21600" windowHeight="11505" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>tidak tersedia PDF, diambil dari tampilan pada situs (pada tanggal 23, jam tidak dicatat).</t>
   </si>
   <si>
-    <t>(diambil pada situs, pada 2020-03-24 16:07 WIB)</t>
-  </si>
-  <si>
     <t>tanggal</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>jumlah_periksa</t>
+  </si>
+  <si>
+    <t>(informasi kasus perawatan diambil pada situs, pada 2020-03-24 16:07 WIB)</t>
   </si>
 </sst>
 </file>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,28 +459,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -1417,7 +1417,7 @@
         <v>43914</v>
       </c>
       <c r="B37">
-        <v>2863</v>
+        <v>3332</v>
       </c>
       <c r="C37">
         <v>686</v>
@@ -1429,7 +1429,7 @@
         <v>55</v>
       </c>
       <c r="F37">
-        <v>2177</v>
+        <v>2625</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -1438,7 +1438,7 @@
         <v>601</v>
       </c>
       <c r="I37" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE: data 25 Maret 2020 21:06 WIB
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C49C4E7-33A5-4D78-9FA8-D312D441AB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720006A-BC7C-4C65-9FA4-D5F930F3DB0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>catatan</t>
   </si>
@@ -74,7 +74,10 @@
     <t>jumlah_periksa</t>
   </si>
   <si>
-    <t>(informasi kasus perawatan diambil pada situs, pada 2020-03-24 16:07 WIB)</t>
+    <t>(informasi diambil di situs, pada 2020-03-25 21:06 WIB)</t>
+  </si>
+  <si>
+    <t>(informasi kasus perawatan diambil di situs, pada 2020-03-24 16:07 WIB)</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,6 +1441,35 @@
         <v>601</v>
       </c>
       <c r="I37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B38">
+        <v>3332</v>
+      </c>
+      <c r="C38">
+        <v>790</v>
+      </c>
+      <c r="D38">
+        <v>31</v>
+      </c>
+      <c r="E38">
+        <v>58</v>
+      </c>
+      <c r="F38">
+        <v>2625</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>701</v>
+      </c>
+      <c r="I38" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UPDATE: kolom positif menjadi konfirmasi
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720006A-BC7C-4C65-9FA4-D5F930F3DB0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E628C1E-4291-4028-A056-10F52FB21E75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>tanggal</t>
   </si>
   <si>
-    <t>positif</t>
-  </si>
-  <si>
     <t>sembuh</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>(informasi kasus perawatan diambil di situs, pada 2020-03-24 16:07 WIB)</t>
+  </si>
+  <si>
+    <t>konfirmasi</t>
   </si>
 </sst>
 </file>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +457,7 @@
     <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -465,25 +465,25 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>601</v>
       </c>
       <c r="I37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>701</v>
       </c>
       <c r="I38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DATA: update 26 Maret 2020
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E628C1E-4291-4028-A056-10F52FB21E75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63236617-161C-4C5A-B034-9930F15DBE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>catatan</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>jumlah_periksa</t>
-  </si>
-  <si>
-    <t>(informasi diambil di situs, pada 2020-03-25 21:06 WIB)</t>
   </si>
   <si>
     <t>(informasi kasus perawatan diambil di situs, pada 2020-03-24 16:07 WIB)</t>
@@ -443,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +465,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -1441,7 +1438,7 @@
         <v>601</v>
       </c>
       <c r="I37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1449,7 +1446,7 @@
         <v>43915</v>
       </c>
       <c r="B38">
-        <v>3332</v>
+        <v>3822</v>
       </c>
       <c r="C38">
         <v>790</v>
@@ -1461,16 +1458,13 @@
         <v>58</v>
       </c>
       <c r="F38">
-        <v>2625</v>
+        <v>3032</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H38">
-        <v>701</v>
-      </c>
-      <c r="I38" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GH: add github action [execnb]
DATA: update 2020-03-30 [execnb]


FIX: GHA [execnb]


FIX: change kernel notebook
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD5EFE6-E02B-462B-A692-C1E97FF70FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2CE546-0BB4-44F3-B4DC-45873E00FCC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>catatan</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>konfirmasi</t>
+  </si>
+  <si>
+    <t>(dari situs)</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,6 +1574,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>43920</v>
+      </c>
+      <c r="B43">
+        <v>6534</v>
+      </c>
+      <c r="C43">
+        <v>1414</v>
+      </c>
+      <c r="D43">
+        <v>122</v>
+      </c>
+      <c r="E43">
+        <v>75</v>
+      </c>
+      <c r="F43">
+        <v>5249</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1107</v>
+      </c>
+      <c r="I43" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
     <sortCondition ref="A2:A36"/>

</xml_diff>

<commit_message>
FIX: remove row 2020-03-30 [execnb]
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2CE546-0BB4-44F3-B4DC-45873E00FCC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6B52A4-7248-432B-90B0-0F319F6AFD27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>catatan</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>konfirmasi</t>
-  </si>
-  <si>
-    <t>(dari situs)</t>
   </si>
 </sst>
 </file>
@@ -441,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,35 +1571,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>43920</v>
-      </c>
-      <c r="B43">
-        <v>6534</v>
-      </c>
-      <c r="C43">
-        <v>1414</v>
-      </c>
-      <c r="D43">
-        <v>122</v>
-      </c>
-      <c r="E43">
-        <v>75</v>
-      </c>
-      <c r="F43">
-        <v>5249</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>1107</v>
-      </c>
-      <c r="I43" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
     <sortCondition ref="A2:A36"/>

</xml_diff>

<commit_message>
DATA: update 2020-03-31 [execnb]
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6B52A4-7248-432B-90B0-0F319F6AFD27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D995A752-5D28-411B-9CAD-A19B87497D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,6 +1571,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>43920</v>
+      </c>
+      <c r="B43">
+        <v>6663</v>
+      </c>
+      <c r="C43">
+        <v>1414</v>
+      </c>
+      <c r="D43">
+        <v>75</v>
+      </c>
+      <c r="E43">
+        <v>122</v>
+      </c>
+      <c r="F43">
+        <v>5249</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
     <sortCondition ref="A2:A36"/>

</xml_diff>

<commit_message>
DATA: update/correction row 2020-03-22 [execnb]
koreksi angka pada tanggal 22 maret berdasarkan blogpost yang tersedia. https://covid19.kemkes.go.id/situasi-infeksi-emerging/info-corona-virus/situasi-terkini-perkembangan-coronavirus-disease-covid-19-23-maret-2020/
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D995A752-5D28-411B-9CAD-A19B87497D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B57E0C0-2EDF-4B51-BCCA-02E4A65ED36A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Tidak tersedia data/Tidak ada perubahan</t>
   </si>
   <si>
-    <t>tidak tersedia PDF, diambil dari tampilan pada situs (pada tanggal 23, jam tidak dicatat).</t>
-  </si>
-  <si>
     <t>tanggal</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>konfirmasi</t>
+  </si>
+  <si>
+    <t>(informasi diperoleh dari blog pos)</t>
   </si>
 </sst>
 </file>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,28 +459,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -1362,28 +1362,28 @@
         <v>43912</v>
       </c>
       <c r="B35">
-        <v>2483</v>
+        <v>2438</v>
       </c>
       <c r="C35">
-        <v>579</v>
+        <v>514</v>
       </c>
       <c r="D35">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E35">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35">
         <v>1904</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H35">
         <v>500</v>
       </c>
       <c r="I35" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>601</v>
       </c>
       <c r="I37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DATA: update 2020-04-01 [execnb]
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B57E0C0-2EDF-4B51-BCCA-02E4A65ED36A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8564C8A0-224F-4CE0-ACEF-4D28E0B291B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,6 +1597,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43921</v>
+      </c>
+      <c r="B44">
+        <v>6777</v>
+      </c>
+      <c r="C44">
+        <v>1528</v>
+      </c>
+      <c r="D44">
+        <v>81</v>
+      </c>
+      <c r="E44">
+        <v>136</v>
+      </c>
+      <c r="F44">
+        <v>5249</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
     <sortCondition ref="A2:A36"/>

</xml_diff>

<commit_message>
DATA: update 2020-04-02 [execnb]
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8564C8A0-224F-4CE0-ACEF-4D28E0B291B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6940E7AA-057D-4D5C-8DFE-08208856B41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,6 +1623,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B45">
+        <v>7193</v>
+      </c>
+      <c r="C45">
+        <v>1677</v>
+      </c>
+      <c r="D45">
+        <v>103</v>
+      </c>
+      <c r="E45">
+        <v>157</v>
+      </c>
+      <c r="F45">
+        <v>5516</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
     <sortCondition ref="A2:A36"/>

</xml_diff>

<commit_message>
DATA: update 2020-04-03 [execnb]
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6940E7AA-057D-4D5C-8DFE-08208856B41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8208E7CB-9D2F-493D-BE6F-1FC59F747F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,6 +1649,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B46">
+        <v>7425</v>
+      </c>
+      <c r="C46">
+        <v>1790</v>
+      </c>
+      <c r="D46">
+        <v>112</v>
+      </c>
+      <c r="E46">
+        <v>170</v>
+      </c>
+      <c r="F46">
+        <v>5635</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
     <sortCondition ref="A2:A36"/>

</xml_diff>

<commit_message>
DATA: update 2020-04-07 [execnb]
</commit_message>
<xml_diff>
--- a/dataset/data_infeksi_covid19_indonesia.xlsx
+++ b/dataset/data_infeksi_covid19_indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\inkovis\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8208E7CB-9D2F-493D-BE6F-1FC59F747F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01C7009-FDB6-4D4B-9C78-6A9263121575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8784433E-335D-44A7-9F88-C2FBB39E525C}"/>
   </bookViews>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CDBA0E-F6EC-436D-A7E0-9B00896D4EF0}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,6 +1675,110 @@
         <v>0</v>
       </c>
     </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B47">
+        <v>7986</v>
+      </c>
+      <c r="C47">
+        <v>1986</v>
+      </c>
+      <c r="D47">
+        <v>134</v>
+      </c>
+      <c r="E47">
+        <v>181</v>
+      </c>
+      <c r="F47">
+        <v>5715</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B48">
+        <v>9712</v>
+      </c>
+      <c r="C48">
+        <v>2092</v>
+      </c>
+      <c r="D48">
+        <v>150</v>
+      </c>
+      <c r="E48">
+        <v>191</v>
+      </c>
+      <c r="F48">
+        <v>7620</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B49">
+        <v>11242</v>
+      </c>
+      <c r="C49">
+        <v>2273</v>
+      </c>
+      <c r="D49">
+        <v>164</v>
+      </c>
+      <c r="E49">
+        <v>198</v>
+      </c>
+      <c r="F49">
+        <v>8869</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B50">
+        <v>13186</v>
+      </c>
+      <c r="C50">
+        <v>2491</v>
+      </c>
+      <c r="D50">
+        <v>192</v>
+      </c>
+      <c r="E50">
+        <v>209</v>
+      </c>
+      <c r="F50">
+        <v>10695</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
     <sortCondition ref="A2:A36"/>

</xml_diff>